<commit_message>
revised (86) we removed med records starting here
</commit_message>
<xml_diff>
--- a/public/templates/healthcard-historical-import-template.xlsx
+++ b/public/templates/healthcard-historical-import-template.xlsx
@@ -399,19 +399,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:A69"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="60.83203125" customWidth="1"/>
+    <col min="1" max="1" width="80.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>HealthCard Historical Data Import Template</v>
+        <v>HEALTHCARD HISTORICAL DATA IMPORT TEMPLATE</v>
       </c>
     </row>
     <row r="2">
@@ -421,153 +419,359 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>INSTRUCTIONS:</v>
+        <v>🚀 QUICK START (FOR TESTING):</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>1. Fill out the "Data" sheet with your historical healthcard statistics</v>
+        <v xml:space="preserve">  You can import this template AS-IS without any changes!</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2. Required fields: Record Date, HealthCard Type, Cards Issued</v>
+        <v xml:space="preserve">  The "Data" sheet contains 8 valid sample records ready for import.</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>3. Optional fields: Barangay, Source, Notes</v>
+        <v xml:space="preserve">  Just click "Import Excel" to test the functionality.</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>4. Valid HealthCard Types: food_handler, non_food, pink</v>
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>5. Date format: YYYY-MM-DD (e.g., 2025-01-15)</v>
+        <v>INSTRUCTIONS FOR REAL DATA:</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>6. Barangay names must match exactly (see "Barangay List" sheet)</v>
+        <v>1. Open the "Data" sheet</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>7. Maximum 1000 records per import</v>
+        <v>2. Delete all sample rows (rows 2-9)</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>8. File size limit: 5MB</v>
+        <v>3. Fill in your actual healthcard data</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v/>
+        <v>4. Maximum 1000 rows per import</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>HEALTHCARD TYPES:</v>
+        <v>5. File size limit: 5MB</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Type</v>
-      </c>
-      <c r="B14" t="str">
-        <v>Display Name</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Description</v>
+        <v>6. Save and import</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>food_handler</v>
-      </c>
-      <c r="B15" t="str">
-        <v>Yellow Card - General</v>
-      </c>
-      <c r="C15" t="str">
-        <v>Health certification for food handlers and restaurant workers</v>
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>non_food</v>
-      </c>
-      <c r="B16" t="str">
-        <v>Green Card - General</v>
-      </c>
-      <c r="C16" t="str">
-        <v>Health certification for non-food industry workers</v>
+        <v>COLUMN DESCRIPTIONS:</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>pink</v>
-      </c>
-      <c r="B17" t="str">
-        <v>Pink Card - Service/Clinical</v>
-      </c>
-      <c r="C17" t="str">
-        <v>Health certification for service and clinical workers</v>
+        <v/>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v/>
+        <v>Record Date (REQUIRED):</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>TIPS:</v>
+        <v xml:space="preserve">  - Format: YYYY-MM-DD (e.g., 2024-01-15)</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>- Leave Barangay blank for system-wide data (not specific to one barangay)</v>
+        <v xml:space="preserve">  - Must be in the past (cannot be future date)</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>- Use Source to track where the data came from (e.g., "CHO Manual Count", "DOH Bulletin")</v>
+        <v xml:space="preserve">  - Excel date format is also supported</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>- Add Notes for any special information about the record</v>
+        <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>- Do not modify column headers in the Data sheet</v>
+        <v>HealthCard Type (REQUIRED):</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v xml:space="preserve">  - Must be one of: food_handler, non_food</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v xml:space="preserve">  - Case-insensitive (e.g., "Food_Handler" or "food_handler" both work)</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v xml:space="preserve">  - food_handler: For food industry workers (restaurants, cafes, food stalls)</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v xml:space="preserve">  - non_food: For non-food industry workers (offices, retail, etc.)</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Cards Issued (REQUIRED):</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v xml:space="preserve">  - Must be a positive integer (1 or greater)</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v xml:space="preserve">  - Number of healthcards issued on this date</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v xml:space="preserve">  - Cannot be 0 or negative</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Barangay (OPTIONAL):</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v xml:space="preserve">  - Must match exact barangay name in the system</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v xml:space="preserve">  - Case-insensitive matching</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v xml:space="preserve">  - Leave blank for system-wide data (no specific barangay)</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v xml:space="preserve">  - Examples: "Datu Abdul Dadia", "San Francisco", "Poblacion"</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v xml:space="preserve">  - See "Barangay List" sheet for valid barangays</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Source (OPTIONAL):</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v xml:space="preserve">  - Reference to data source</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v xml:space="preserve">  - Examples: "CHO Manual Count", "DOH Bulletin", "CHO Records"</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v xml:space="preserve">  - Useful for audit trail and data provenance</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Notes (OPTIONAL):</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v xml:space="preserve">  - Additional information or comments</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v xml:space="preserve">  - Any relevant details about this record</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v xml:space="preserve">  - Examples: "January batch", "Q1 2024 data", "Walk-in processing"</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>VALIDATION RULES:</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v xml:space="preserve">  ✓ All dates must be in the past</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v xml:space="preserve">  ✓ Cards Issued must be &gt; 0 (positive integer)</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v xml:space="preserve">  ✓ HealthCard Type must be "food_handler" or "non_food"</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v xml:space="preserve">  ✓ Barangay name must exist in system (if provided)</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v xml:space="preserve">  ✓ Maximum 1000 records per import</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v xml:space="preserve">  ✓ File size must be under 5MB</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>ERROR HANDLING:</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v xml:space="preserve">  - The import will show detailed validation errors</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v xml:space="preserve">  - Errors include row number and specific field issues</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v xml:space="preserve">  - Fix all errors before importing</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v xml:space="preserve">  - Only valid records will be imported</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>EXAMPLE USE CASES:</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v xml:space="preserve">  1. Historical CHO records digitization</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v xml:space="preserve">  2. DOH regional data consolidation</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v xml:space="preserve">  3. Monthly/quarterly batch imports</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v xml:space="preserve">  4. Training data for SARIMA prediction models</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A69"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" customWidth="1"/>
-    <col min="6" max="6" width="40.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" customWidth="1"/>
+    <col min="6" max="6" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -592,608 +796,479 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-01-15</v>
+        <v>2020-03-15</v>
       </c>
       <c r="B2" t="str">
         <v>food_handler</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2">
         <v>45</v>
       </c>
       <c r="D2" t="str">
-        <v>Dapco</v>
+        <v>Datu Abdul Dadia</v>
       </c>
       <c r="E2" t="str">
-        <v>CHO Manual Count</v>
+        <v>CHO Manual Records</v>
       </c>
       <c r="F2" t="str">
-        <v>Regular monthly count</v>
+        <v>Q1 2020 - Pre-pandemic batch</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-01-10</v>
+        <v>2020-06-10</v>
       </c>
       <c r="B3" t="str">
         <v>non_food</v>
       </c>
-      <c r="C3" t="str">
-        <v>23</v>
+      <c r="C3">
+        <v>32</v>
       </c>
       <c r="D3" t="str">
         <v>Gredu</v>
       </c>
       <c r="E3" t="str">
-        <v>CHO Database Export</v>
+        <v>CHO Manual Records</v>
       </c>
       <c r="F3" t="str">
-        <v>Including backlog entries</v>
+        <v>Q2 2020 - Limited operations due to COVID-19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-01-08</v>
+        <v>2020-09-20</v>
       </c>
       <c r="B4" t="str">
-        <v>pink</v>
-      </c>
-      <c r="C4" t="str">
-        <v>12</v>
+        <v>food_handler</v>
+      </c>
+      <c r="C4">
+        <v>38</v>
       </c>
       <c r="D4" t="str">
-        <v>New Pandan</v>
+        <v/>
       </c>
       <c r="E4" t="str">
-        <v>CHO Manual Count</v>
+        <v>DOH Regional Data</v>
       </c>
       <c r="F4" t="str">
-        <v>Service workers certification</v>
+        <v>Q3 2020 - Gradual reopening of food establishments</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>2024-12-20</v>
+        <v>2020-12-05</v>
       </c>
       <c r="B5" t="str">
-        <v>food_handler</v>
-      </c>
-      <c r="C5" t="str">
-        <v>67</v>
+        <v>non_food</v>
+      </c>
+      <c r="C5">
+        <v>28</v>
       </c>
       <c r="D5" t="str">
         <v/>
       </c>
       <c r="E5" t="str">
-        <v>DOH Bulletin</v>
+        <v>CHO Manual Records</v>
       </c>
       <c r="F5" t="str">
-        <v>System-wide data (no specific barangay)</v>
+        <v>Q4 2020 - Year-end processing</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>2024-12-15</v>
+        <v>2021-02-14</v>
       </c>
       <c r="B6" t="str">
-        <v>non_food</v>
-      </c>
-      <c r="C6" t="str">
-        <v>34</v>
+        <v>food_handler</v>
+      </c>
+      <c r="C6">
+        <v>52</v>
       </c>
       <c r="D6" t="str">
-        <v>Poblacion</v>
+        <v>New Pandan (Poblacion)</v>
       </c>
       <c r="E6" t="str">
-        <v>CHO Records</v>
+        <v>CHO Manual Records</v>
       </c>
       <c r="F6" t="str">
-        <v/>
+        <v>Q1 2021 - Recovery period processing</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>2024-12-10</v>
+        <v>2021-05-22</v>
       </c>
       <c r="B7" t="str">
-        <v>pink</v>
-      </c>
-      <c r="C7" t="str">
-        <v>18</v>
+        <v>non_food</v>
+      </c>
+      <c r="C7">
+        <v>41</v>
       </c>
       <c r="D7" t="str">
+        <v>San Francisco (Poblacion)</v>
+      </c>
+      <c r="E7" t="str">
+        <v>DOH Regional Data</v>
+      </c>
+      <c r="F7" t="str">
+        <v>Q2 2021 - Increased applications</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>2021-08-18</v>
+      </c>
+      <c r="B8" t="str">
+        <v>food_handler</v>
+      </c>
+      <c r="C8">
+        <v>47</v>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <v>CHO Manual Records</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Q3 2021 - Surge in food handler certifications</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>2021-11-10</v>
+      </c>
+      <c r="B9" t="str">
+        <v>non_food</v>
+      </c>
+      <c r="C9">
+        <v>35</v>
+      </c>
+      <c r="D9" t="str">
         <v>Kasilak</v>
       </c>
-      <c r="E7" t="str">
-        <v>CHO Manual Count</v>
-      </c>
-      <c r="F7" t="str">
-        <v>Clinical workers health screening</v>
+      <c r="E9" t="str">
+        <v>CHO Manual Records</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Q4 2021 - Year-end batch</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>2022-01-25</v>
+      </c>
+      <c r="B10" t="str">
+        <v>food_handler</v>
+      </c>
+      <c r="C10">
+        <v>58</v>
+      </c>
+      <c r="D10" t="str">
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <v>CHO Manual Records</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Q1 2022 - High demand from restaurants</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>2022-04-12</v>
+      </c>
+      <c r="B11" t="str">
+        <v>non_food</v>
+      </c>
+      <c r="C11">
+        <v>44</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Dapco</v>
+      </c>
+      <c r="E11" t="str">
+        <v>DOH Regional Data</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Q2 2022 - Office workers returning</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>2022-07-08</v>
+      </c>
+      <c r="B12" t="str">
+        <v>food_handler</v>
+      </c>
+      <c r="C12">
+        <v>63</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Mabunao</v>
+      </c>
+      <c r="E12" t="str">
+        <v>CHO Manual Records</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Q3 2022 - Peak season processing</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>2022-10-15</v>
+      </c>
+      <c r="B13" t="str">
+        <v>non_food</v>
+      </c>
+      <c r="C13">
+        <v>39</v>
+      </c>
+      <c r="D13" t="str">
+        <v/>
+      </c>
+      <c r="E13" t="str">
+        <v>CHO Manual Records</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Q4 2022 - Final pre-system batch</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F13"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:A43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="1" max="1" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Barangay Name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Code</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Notes</v>
+        <v>VALID BARANGAY NAMES</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>A. O. Floirendo</v>
-      </c>
-      <c r="B2" t="str">
-        <v>AOF</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Use exact name when importing</v>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Dapco</v>
-      </c>
-      <c r="B3" t="str">
-        <v>DAP</v>
-      </c>
-      <c r="C3" t="str">
-        <v/>
+        <v>Use these exact names in the "Barangay" column:</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Gredu</v>
-      </c>
-      <c r="B4" t="str">
-        <v>GRE</v>
-      </c>
-      <c r="C4" t="str">
-        <v/>
+        <v>(Leave blank for system-wide data)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>J.P. Laurel</v>
-      </c>
-      <c r="B5" t="str">
-        <v>JPL</v>
-      </c>
-      <c r="C5" t="str">
         <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Kasilak</v>
-      </c>
-      <c r="B6" t="str">
-        <v>KAS</v>
-      </c>
-      <c r="C6" t="str">
-        <v/>
+        <v>A. O. Floirendo</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Katipunan</v>
-      </c>
-      <c r="B7" t="str">
-        <v>KAT</v>
-      </c>
-      <c r="C7" t="str">
-        <v/>
+        <v>Buenavista</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Kauswagan</v>
-      </c>
-      <c r="B8" t="str">
-        <v>KAU</v>
-      </c>
-      <c r="C8" t="str">
-        <v/>
+        <v>Cacao</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Katualan</v>
-      </c>
-      <c r="B9" t="str">
-        <v>KAA</v>
-      </c>
-      <c r="C9" t="str">
-        <v/>
+        <v>Cagangohan</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Kiotoy</v>
-      </c>
-      <c r="B10" t="str">
-        <v>KIO</v>
-      </c>
-      <c r="C10" t="str">
-        <v/>
+        <v>Consolacion</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Lower Licanan</v>
-      </c>
-      <c r="B11" t="str">
-        <v>LLI</v>
-      </c>
-      <c r="C11" t="str">
-        <v/>
+        <v>Dapco</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Mabunao</v>
-      </c>
-      <c r="B12" t="str">
-        <v>MAB</v>
-      </c>
-      <c r="C12" t="str">
-        <v/>
+        <v>Datu Abdul Dadia</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Maduao</v>
-      </c>
-      <c r="B13" t="str">
-        <v>MAD</v>
-      </c>
-      <c r="C13" t="str">
-        <v/>
+        <v>Gredu</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Malativas</v>
-      </c>
-      <c r="B14" t="str">
-        <v>MAL</v>
-      </c>
-      <c r="C14" t="str">
-        <v/>
+        <v>J.P. Laurel</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Manay</v>
-      </c>
-      <c r="B15" t="str">
-        <v>MAN</v>
-      </c>
-      <c r="C15" t="str">
-        <v/>
+        <v>Kasilak</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Nanyo</v>
-      </c>
-      <c r="B16" t="str">
-        <v>NAN</v>
-      </c>
-      <c r="C16" t="str">
-        <v/>
+        <v>Katipunan</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>New Malaga</v>
-      </c>
-      <c r="B17" t="str">
-        <v>NMA</v>
-      </c>
-      <c r="C17" t="str">
-        <v/>
+        <v>Katualan</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>New Malitbog</v>
-      </c>
-      <c r="B18" t="str">
-        <v>NMB</v>
-      </c>
-      <c r="C18" t="str">
-        <v/>
+        <v>Kauswagan</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>New Pandan</v>
-      </c>
-      <c r="B19" t="str">
-        <v>NPA</v>
-      </c>
-      <c r="C19" t="str">
-        <v/>
+        <v>Kiotoy</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>New Visayas</v>
-      </c>
-      <c r="B20" t="str">
-        <v>NVI</v>
-      </c>
-      <c r="C20" t="str">
-        <v/>
+        <v>Little Panay</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Poblacion</v>
-      </c>
-      <c r="B21" t="str">
-        <v>POB</v>
-      </c>
-      <c r="C21" t="str">
-        <v/>
+        <v>Lower Panaga (Roxas)</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>San Francisco</v>
-      </c>
-      <c r="B22" t="str">
-        <v>SFR</v>
-      </c>
-      <c r="C22" t="str">
-        <v/>
+        <v>Mabunao</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>San Nicolas</v>
-      </c>
-      <c r="B23" t="str">
-        <v>SNI</v>
-      </c>
-      <c r="C23" t="str">
-        <v/>
+        <v>Maduao</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>San Pedro</v>
-      </c>
-      <c r="B24" t="str">
-        <v>SPE</v>
-      </c>
-      <c r="C24" t="str">
-        <v/>
+        <v>Malativas</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>San Roque</v>
-      </c>
-      <c r="B25" t="str">
-        <v>SRO</v>
-      </c>
-      <c r="C25" t="str">
-        <v/>
+        <v>Manay</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>San Vicente</v>
-      </c>
-      <c r="B26" t="str">
-        <v>SVI</v>
-      </c>
-      <c r="C26" t="str">
-        <v/>
+        <v>Nanyo</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Santa Cruz</v>
-      </c>
-      <c r="B27" t="str">
-        <v>SCR</v>
-      </c>
-      <c r="C27" t="str">
-        <v/>
+        <v>New Malaga (New Malitbog)</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Santo Niño</v>
-      </c>
-      <c r="B28" t="str">
-        <v>SNO</v>
-      </c>
-      <c r="C28" t="str">
-        <v/>
+        <v>New Pandan (Poblacion)</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Sindaton</v>
-      </c>
-      <c r="B29" t="str">
-        <v>SIN</v>
-      </c>
-      <c r="C29" t="str">
-        <v/>
+        <v>New Visayas</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Southern Davao</v>
-      </c>
-      <c r="B30" t="str">
-        <v>SDA</v>
-      </c>
-      <c r="C30" t="str">
-        <v/>
+        <v>Quezon</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Tibungol</v>
-      </c>
-      <c r="B31" t="str">
-        <v>TIB</v>
-      </c>
-      <c r="C31" t="str">
-        <v/>
+        <v>Salvacion</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Upper Licanan</v>
-      </c>
-      <c r="B32" t="str">
-        <v>ULI</v>
-      </c>
-      <c r="C32" t="str">
-        <v/>
+        <v>San Francisco (Poblacion)</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Waterfall</v>
-      </c>
-      <c r="B33" t="str">
-        <v>WAT</v>
-      </c>
-      <c r="C33" t="str">
-        <v/>
+        <v>San Nicolas</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Buenavista</v>
-      </c>
-      <c r="B34" t="str">
-        <v>BUE</v>
-      </c>
-      <c r="C34" t="str">
-        <v/>
+        <v>San Pedro</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Cacao</v>
-      </c>
-      <c r="B35" t="str">
-        <v>CAC</v>
-      </c>
-      <c r="C35" t="str">
-        <v/>
+        <v>San Roque</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Consolacion</v>
-      </c>
-      <c r="B36" t="str">
-        <v>CON</v>
-      </c>
-      <c r="C36" t="str">
-        <v/>
+        <v>San Vicente</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Datu Balong</v>
-      </c>
-      <c r="B37" t="str">
-        <v>DBA</v>
-      </c>
-      <c r="C37" t="str">
-        <v/>
+        <v>Santa Cruz</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Little Panay</v>
-      </c>
-      <c r="B38" t="str">
-        <v>LPA</v>
-      </c>
-      <c r="C38" t="str">
-        <v/>
+        <v>Santo Niño (Poblacion)</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>Lower Panaga</v>
-      </c>
-      <c r="B39" t="str">
-        <v>LPG</v>
-      </c>
-      <c r="C39" t="str">
-        <v/>
+        <v>Sindaton</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Magsaysay</v>
-      </c>
-      <c r="B40" t="str">
-        <v>MAG</v>
-      </c>
-      <c r="C40" t="str">
-        <v/>
+        <v>Southern Davao</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Quezon</v>
-      </c>
-      <c r="B41" t="str">
-        <v>QUE</v>
-      </c>
-      <c r="C41" t="str">
-        <v/>
+        <v>Tagpore</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Salvacion</v>
-      </c>
-      <c r="B42" t="str">
-        <v>SAL</v>
-      </c>
-      <c r="C42" t="str">
-        <v/>
+        <v>Tibungol</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Upper Licanan</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C42"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A43"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>